<commit_message>
third train: edit vector, with last, last2(best performance)
ngram on train
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="150" firstSheet="0" activeTab="0"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>algo</t>
   </si>
@@ -66,6 +66,27 @@
   </si>
   <si>
     <t>Symspell + prefix</t>
+  </si>
+  <si>
+    <t>cover rate</t>
+  </si>
+  <si>
+    <t>neg:pos</t>
+  </si>
+  <si>
+    <t>bigram</t>
+  </si>
+  <si>
+    <t>Edit 2</t>
+  </si>
+  <si>
+    <t>Edit 1</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>part2</t>
   </si>
 </sst>
 </file>
@@ -161,10 +182,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -333,6 +354,120 @@
         <v>0.186297667901</v>
       </c>
     </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>0.845581022921</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>277.483321891</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>0.793564207787</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>27.1586933216</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>92595</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>99910</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>0.926784105695</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>831940</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>900090</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>0.924285349243</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>93066</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>99910</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>0.931498348514</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>837860</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>900090</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>0.930862469309</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
remember mistake + edit distance edit operation param optimization is running
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="150" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="146" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>algo</t>
   </si>
@@ -38,6 +38,9 @@
     <t>contain</t>
   </si>
   <si>
+    <t>test</t>
+  </si>
+  <si>
     <t>symspell</t>
   </si>
   <si>
@@ -68,12 +71,24 @@
     <t>Symspell + prefix</t>
   </si>
   <si>
+    <t>word embed</t>
+  </si>
+  <si>
+    <t>part1.part1</t>
+  </si>
+  <si>
+    <t>part1.part2</t>
+  </si>
+  <si>
     <t>cover rate</t>
   </si>
   <si>
     <t>neg:pos</t>
   </si>
   <si>
+    <t>trigram</t>
+  </si>
+  <si>
     <t>bigram</t>
   </si>
   <si>
@@ -83,7 +98,25 @@
     <t>Edit 1</t>
   </si>
   <si>
-    <t>test</t>
+    <t>Bigram(500)</t>
+  </si>
+  <si>
+    <t>Bigram(100)</t>
+  </si>
+  <si>
+    <t>Bigram(1000)</t>
+  </si>
+  <si>
+    <t>bigram(edit1)</t>
+  </si>
+  <si>
+    <t>edit1(kb)</t>
+  </si>
+  <si>
+    <t>edit2(kb)</t>
+  </si>
+  <si>
+    <t>edit3(kb)</t>
   </si>
   <si>
     <t>part2</t>
@@ -101,6 +134,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -182,16 +216,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.2244897959184"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -216,16 +252,19 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0.709488539686</v>
@@ -236,7 +275,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0.712631368231</v>
@@ -247,7 +286,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>0.713352016815</v>
@@ -258,7 +297,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>0.713602242018</v>
@@ -269,7 +308,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>0.713942548293</v>
@@ -280,7 +319,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>0.713231908718</v>
@@ -291,7 +330,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>0.711190071064</v>
@@ -302,10 +341,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>0.723441096987</v>
@@ -322,7 +361,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>0.723521169052</v>
@@ -339,7 +378,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>0.722360124112</v>
@@ -354,117 +393,236 @@
         <v>0.186297667901</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>0.645647457725</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D17" s="0" t="n">
+        <v>0.646880258686</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>0.79</v>
+        <v>0.153067760985</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>13275.6168835</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>0.845581022921</v>
+        <v>0.875618056251</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>277.483321891</v>
+        <v>30243.0598173</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B26" s="0" t="n">
+        <v>0.845581022921</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>277.483321891</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="n">
         <v>0.793564207787</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C27" s="0" t="n">
         <v>27.1586933216</v>
       </c>
     </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>0.773416074467</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>460.94427477</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>0.634841357221</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>96.9609156984</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>0.809328395556</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>875.666398714</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>0.743829446502</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>14.584517466</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>0.74008607747</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>8.41379730059</v>
+      </c>
+    </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
+      <c r="A33" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>0.783415073566</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>43.3566966054</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>0.808477629867</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>114.570077375</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D34" s="0" t="n">
+      <c r="C38" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="0" t="n">
         <v>92595</v>
       </c>
-      <c r="E34" s="0" t="n">
+      <c r="E39" s="0" t="n">
         <v>99910</v>
       </c>
-      <c r="F34" s="0" t="n">
+      <c r="F39" s="0" t="n">
         <v>0.926784105695</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D35" s="0" t="n">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40" s="0" t="n">
         <v>831940</v>
       </c>
-      <c r="E35" s="0" t="n">
+      <c r="E40" s="0" t="n">
         <v>900090</v>
       </c>
-      <c r="F35" s="0" t="n">
+      <c r="F40" s="0" t="n">
         <v>0.924285349243</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" s="0" t="n">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="0" t="n">
         <v>93066</v>
       </c>
-      <c r="E36" s="0" t="n">
+      <c r="E41" s="0" t="n">
         <v>99910</v>
       </c>
-      <c r="F36" s="0" t="n">
+      <c r="F41" s="0" t="n">
         <v>0.931498348514</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D37" s="0" t="n">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="0" t="n">
         <v>837860</v>
       </c>
-      <c r="E37" s="0" t="n">
+      <c r="E42" s="0" t="n">
         <v>900090</v>
       </c>
-      <c r="F37" s="0" t="n">
+      <c r="F42" s="0" t="n">
         <v>0.930862469309</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finish, cis accuracy: 83%, cs accuracy: 76%
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="146" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="142" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>algo</t>
   </si>
@@ -120,6 +120,15 @@
   </si>
   <si>
     <t>part2</t>
+  </si>
+  <si>
+    <t>case sensitive</t>
+  </si>
+  <si>
+    <t>accuracy on train</t>
+  </si>
+  <si>
+    <t>accuracy on test</t>
   </si>
 </sst>
 </file>
@@ -216,16 +225,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.2244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3877551020408"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1377551020408"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
@@ -624,6 +633,17 @@
       </c>
       <c r="F42" s="0" t="n">
         <v>0.930862469309</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>